<commit_message>
Missing pointers for all types of insurance
</commit_message>
<xml_diff>
--- a/Attribute_List_Marine.xlsx
+++ b/Attribute_List_Marine.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="202">
   <si>
     <t>Path</t>
   </si>
@@ -87,13 +87,13 @@
     <t>https://www.abcinsurance.com/content/dam/abcinsurance/india/assets/images/header/logo.png</t>
   </si>
   <si>
-    <t>Physical description of insurer</t>
+    <t>Logo of insurer</t>
   </si>
   <si>
     <t>message.catalog.providers.descriptor.image.size_type</t>
   </si>
   <si>
-    <t>optional</t>
+    <t>Optional</t>
   </si>
   <si>
     <t>sm</t>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>message.catalog.providers.descriptor.short_desc</t>
+  </si>
+  <si>
+    <t>optional</t>
   </si>
   <si>
     <t>Short description about insurer</t>
@@ -174,19 +177,19 @@
     <t>number</t>
   </si>
   <si>
-    <t>Minimum index value of form</t>
+    <t>Minimum number of pages in a form</t>
   </si>
   <si>
     <t>message.catalog.provider.item.xinput.head.index.max</t>
   </si>
   <si>
-    <t>Maximum index value of form</t>
+    <t>Maximum number of pages in a form</t>
   </si>
   <si>
     <t>message.catalog.provider.item.xinput.head.index.cur</t>
   </si>
   <si>
-    <t>Current index value of form</t>
+    <t>Current page to be filled in a form</t>
   </si>
   <si>
     <t>message.catalog.provider.item.xinput.head.headings</t>
@@ -312,10 +315,16 @@
     <t>ABC Marine Insurance Policy</t>
   </si>
   <si>
+    <t>Name of the insurance item</t>
+  </si>
+  <si>
     <t>message.order.items.descriptor.short_des</t>
   </si>
   <si>
     <t>ABC Marine Insurance Class A</t>
+  </si>
+  <si>
+    <t>Short description about the item</t>
   </si>
   <si>
     <t>message.order.items.id</t>
@@ -361,9 +370,6 @@
   </si>
   <si>
     <t>message.order.provider.descriptor.long_desc</t>
-  </si>
-  <si>
-    <t>Optional</t>
   </si>
   <si>
     <t>ABC Insurance Ltd. Deals in multiple Insurance Services like Health,
@@ -421,7 +427,7 @@
     <t>Coverage Time</t>
   </si>
   <si>
-    <t>Validity of insurance policy</t>
+    <t>Label value of the time</t>
   </si>
   <si>
     <t>message.order.items.time.range.start</t>
@@ -523,13 +529,13 @@
     <t>message.order.price.value</t>
   </si>
   <si>
-    <t>Value of order price</t>
+    <t>Value of the order price</t>
   </si>
   <si>
     <t>message.order.fulfillments.person.dob</t>
   </si>
   <si>
-    <t>Date of birth of person</t>
+    <t>Date of birth of the person</t>
   </si>
   <si>
     <t>message.order.fulfillments.person.gender</t>
@@ -538,7 +544,7 @@
     <t>male</t>
   </si>
   <si>
-    <t>Gender of person</t>
+    <t>Gender of the person</t>
   </si>
   <si>
     <t>message.order.fulfillments.organization.address</t>
@@ -559,6 +565,9 @@
     <t>message.order.quote.price.currency</t>
   </si>
   <si>
+    <t>Currency of the order price</t>
+  </si>
+  <si>
     <t>PRE-ORDER</t>
   </si>
   <si>
@@ -566,6 +575,9 @@
   </si>
   <si>
     <t>2023-07-01T07:12:47.419Z</t>
+  </si>
+  <si>
+    <t>Value of the price</t>
   </si>
   <si>
     <t>message.order.id</t>
@@ -583,7 +595,10 @@
     <t>ACTIVE</t>
   </si>
   <si>
-    <t>Status of order</t>
+    <t>Status of the order</t>
+  </si>
+  <si>
+    <t>Date of birth of person</t>
   </si>
   <si>
     <t>message.order.payments.url</t>
@@ -614,6 +629,12 @@
   </si>
   <si>
     <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>Status of order</t>
+  </si>
+  <si>
+    <t>Phone number of the contact</t>
   </si>
   <si>
     <t>Refund Amount</t>
@@ -712,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -782,6 +803,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -4128,7 +4152,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -4136,7 +4160,7 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -4148,15 +4172,15 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -4168,35 +4192,35 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -4208,15 +4232,15 @@
         <v>13</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -4228,15 +4252,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -4247,16 +4271,16 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="26">
         <v>32894.0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -4268,15 +4292,15 @@
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -4288,15 +4312,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -4308,15 +4332,15 @@
         <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -4328,7 +4352,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>18</v>
@@ -4336,13 +4360,13 @@
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -4351,12 +4375,12 @@
         <v>1000.0</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
@@ -4368,15 +4392,15 @@
         <v>13</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -4388,21 +4412,21 @@
         <v>13</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -4411,12 +4435,12 @@
         <v>900.0</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
@@ -4428,15 +4452,15 @@
         <v>13</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -4448,15 +4472,15 @@
         <v>13</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -4468,21 +4492,21 @@
         <v>13</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>13</v>
@@ -4491,18 +4515,18 @@
         <v>13</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>13</v>
@@ -4511,18 +4535,18 @@
         <v>100000.0</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>13</v>
@@ -4531,12 +4555,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
@@ -4548,15 +4572,15 @@
         <v>13</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>7</v>
@@ -4567,16 +4591,16 @@
       <c r="D23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>151</v>
+      <c r="E23" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -4588,15 +4612,15 @@
         <v>13</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>7</v>
@@ -4608,18 +4632,18 @@
         <v>13</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>8</v>
@@ -4628,15 +4652,15 @@
         <v>13</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>7</v>
@@ -4648,7 +4672,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>28</v>
@@ -4656,10 +4680,10 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>8</v>
@@ -4668,10 +4692,10 @@
         <v>13</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
@@ -4767,7 +4791,7 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -4778,16 +4802,16 @@
       <c r="D2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="28">
         <v>1.0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="11" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -4802,7 +4826,7 @@
         <v>5.0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4839,7 +4863,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -4847,7 +4871,7 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -4859,15 +4883,15 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -4879,35 +4903,35 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -4919,15 +4943,15 @@
         <v>13</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -4939,15 +4963,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -4958,16 +4982,16 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="26">
         <v>32894.0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -4979,15 +5003,15 @@
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -4999,15 +5023,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -5019,7 +5043,7 @@
         <v>13</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>18</v>
@@ -5027,7 +5051,7 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -5039,21 +5063,21 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>13</v>
@@ -5062,12 +5086,12 @@
         <v>0.0</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
@@ -5079,15 +5103,15 @@
         <v>13</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -5099,15 +5123,15 @@
         <v>13</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -5119,21 +5143,21 @@
         <v>13</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -5142,18 +5166,18 @@
         <v>13</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>13</v>
@@ -5162,18 +5186,18 @@
         <v>100000.0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>13</v>
@@ -5182,12 +5206,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -5199,15 +5223,15 @@
         <v>13</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -5218,16 +5242,16 @@
       <c r="D20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>151</v>
+      <c r="E20" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
@@ -5239,15 +5263,15 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
@@ -5259,18 +5283,18 @@
         <v>13</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
@@ -5279,15 +5303,15 @@
         <v>13</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>7</v>
@@ -5299,7 +5323,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>28</v>
@@ -5307,10 +5331,10 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -5319,10 +5343,10 @@
         <v>13</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26">
@@ -5509,7 +5533,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -5521,15 +5545,15 @@
         <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -5541,12 +5565,12 @@
         <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -5558,15 +5582,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -5578,15 +5602,15 @@
         <v>13</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -5598,15 +5622,15 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -5618,21 +5642,21 @@
         <v>13</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -5641,18 +5665,18 @@
         <v>0.0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -5661,18 +5685,18 @@
         <v>0.0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -5681,12 +5705,12 @@
         <v>0.0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
@@ -5698,15 +5722,15 @@
         <v>13</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -5718,15 +5742,15 @@
         <v>13</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -5738,15 +5762,15 @@
         <v>13</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -5758,21 +5782,21 @@
         <v>13</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -5781,18 +5805,18 @@
         <v>0</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -5801,18 +5825,18 @@
         <v>0</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
@@ -5821,7 +5845,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23">
@@ -9767,7 +9791,7 @@
     </row>
     <row r="2">
       <c r="A2" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -9779,15 +9803,15 @@
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -9799,15 +9823,15 @@
         <v>9</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -9819,10 +9843,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -9847,7 +9871,7 @@
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -9859,10 +9883,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
@@ -9887,7 +9911,7 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -9899,15 +9923,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -9919,15 +9943,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -13974,7 +13998,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -13986,15 +14010,15 @@
         <v>13</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -14006,15 +14030,15 @@
         <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -14026,15 +14050,15 @@
         <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -14046,15 +14070,15 @@
         <v>13</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -14066,21 +14090,21 @@
         <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -14089,18 +14113,18 @@
         <v>0.0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -14109,18 +14133,18 @@
         <v>1.0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -14129,12 +14153,12 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -14146,15 +14170,15 @@
         <v>13</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -14166,15 +14190,15 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -14186,21 +14210,21 @@
         <v>13</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -14209,18 +14233,18 @@
         <v>1</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -14229,18 +14253,18 @@
         <v>0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -14249,15 +14273,15 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -14266,15 +14290,15 @@
         <v>13</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -14286,7 +14310,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>28</v>
@@ -14294,10 +14318,10 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -14306,15 +14330,15 @@
         <v>13</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>7</v>
@@ -14326,7 +14350,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>21</v>
@@ -14334,7 +14358,7 @@
     </row>
     <row r="20">
       <c r="A20" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>7</v>
@@ -14354,13 +14378,13 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -14369,12 +14393,12 @@
         <v>900.0</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
@@ -14386,10 +14410,10 @@
         <v>13</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -18344,27 +18368,27 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -18376,15 +18400,15 @@
         <v>9</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -18396,15 +18420,15 @@
         <v>9</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -18416,15 +18440,15 @@
         <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -18436,15 +18460,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -18456,15 +18480,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -18476,15 +18500,15 @@
         <v>9</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -18496,15 +18520,15 @@
         <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -18516,15 +18540,15 @@
         <v>9</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -18536,21 +18560,21 @@
         <v>9</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
@@ -18559,18 +18583,18 @@
         <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
@@ -18579,18 +18603,18 @@
         <v>1000.0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -18599,12 +18623,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -18616,15 +18640,15 @@
         <v>9</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
@@ -18635,16 +18659,16 @@
       <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>151</v>
+      <c r="E16" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -18656,15 +18680,15 @@
         <v>9</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -18676,15 +18700,15 @@
         <v>9</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -18704,7 +18728,7 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -18719,12 +18743,12 @@
         <v>90000.0</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
@@ -18736,15 +18760,15 @@
         <v>9</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
@@ -18756,21 +18780,21 @@
         <v>9</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
@@ -18779,7 +18803,7 @@
         <v>100000.0</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24">
@@ -21760,27 +21784,27 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -21792,15 +21816,15 @@
         <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -21812,15 +21836,15 @@
         <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -21831,16 +21855,16 @@
       <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="26">
         <v>32894.0</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -21852,15 +21876,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -21872,15 +21896,15 @@
         <v>13</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="26" t="s">
-        <v>89</v>
+      <c r="A8" s="27" t="s">
+        <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -21892,15 +21916,15 @@
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -21912,7 +21936,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>18</v>
@@ -21920,13 +21944,13 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>13</v>
@@ -21935,12 +21959,12 @@
         <v>1000.0</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -21952,15 +21976,15 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -21972,21 +21996,21 @@
         <v>13</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>13</v>
@@ -21995,18 +22019,18 @@
         <v>900.0</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>13</v>
@@ -22015,18 +22039,18 @@
         <v>13</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -22035,18 +22059,18 @@
         <v>1000.0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -22055,12 +22079,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -22072,15 +22096,15 @@
         <v>13</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -22091,16 +22115,16 @@
       <c r="D18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>151</v>
+      <c r="E18" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -22112,15 +22136,15 @@
         <v>13</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -22132,10 +22156,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21">
@@ -26032,7 +26056,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -26040,27 +26064,27 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -26072,15 +26096,15 @@
         <v>9</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -26092,15 +26116,15 @@
         <v>9</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -26112,15 +26136,15 @@
         <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -26132,15 +26156,15 @@
         <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -26152,15 +26176,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -26172,15 +26196,15 @@
         <v>9</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -26192,21 +26216,21 @@
         <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
@@ -26215,18 +26239,18 @@
         <v>13</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>9</v>
@@ -26235,18 +26259,18 @@
         <v>1000.0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
@@ -26255,12 +26279,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
@@ -26272,15 +26296,15 @@
         <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -26291,16 +26315,16 @@
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>151</v>
+      <c r="E14" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -26312,15 +26336,15 @@
         <v>9</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
@@ -26332,15 +26356,15 @@
         <v>9</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -26352,7 +26376,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>18</v>
@@ -26360,13 +26384,13 @@
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
@@ -26375,12 +26399,12 @@
         <v>1000.0</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -26392,15 +26416,15 @@
         <v>9</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -26412,21 +26436,21 @@
         <v>9</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -26435,7 +26459,7 @@
         <v>900.0</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -26475,7 +26499,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -26483,7 +26507,7 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -26495,15 +26519,15 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -26515,35 +26539,35 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -26555,15 +26579,15 @@
         <v>13</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -26575,15 +26599,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -26594,16 +26618,16 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="26">
         <v>32894.0</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -26615,15 +26639,15 @@
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -26635,15 +26659,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -26655,15 +26679,15 @@
         <v>13</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -26675,15 +26699,15 @@
         <v>13</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -26695,15 +26719,15 @@
         <v>13</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
@@ -26715,21 +26739,21 @@
         <v>13</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>13</v>
@@ -26738,18 +26762,18 @@
         <v>13</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>13</v>
@@ -26758,18 +26782,18 @@
         <v>100000.0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>13</v>
@@ -26778,12 +26802,12 @@
         <v>1.800002341E9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -26795,15 +26819,15 @@
         <v>13</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -26814,16 +26838,16 @@
       <c r="D18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>151</v>
+      <c r="E18" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -26835,15 +26859,15 @@
         <v>13</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -26855,18 +26879,18 @@
         <v>13</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>8</v>
@@ -26875,15 +26899,15 @@
         <v>13</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
@@ -26895,7 +26919,7 @@
         <v>13</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>28</v>
@@ -26903,10 +26927,10 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
@@ -26915,10 +26939,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -26959,7 +26983,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -26967,7 +26991,7 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -26978,11 +27002,11 @@
       <c r="D2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="28">
         <v>1.0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>